<commit_message>
added margin win for new leagues
</commit_message>
<xml_diff>
--- a/Divisions/D1.xlsx
+++ b/Divisions/D1.xlsx
@@ -780,382 +780,382 @@
     <t>Team against</t>
   </si>
   <si>
-    <t>Augsburg,L D W L L D</t>
-  </si>
-  <si>
-    <t>Bayern Munich,W W W W L W</t>
-  </si>
-  <si>
-    <t>Bielefeld,D L D L L D</t>
-  </si>
-  <si>
-    <t>Bochum,L L L D L W</t>
-  </si>
-  <si>
-    <t>Dortmund,W W W L W W</t>
-  </si>
-  <si>
-    <t>Ein Frankfurt,D D D D W L</t>
-  </si>
-  <si>
-    <t>FC Koln,W D D D W L</t>
-  </si>
-  <si>
-    <t>Freiburg,W D D W W D</t>
-  </si>
-  <si>
-    <t>Greuther Furth,L L L L L L</t>
-  </si>
-  <si>
-    <t>Hertha,L W W L L W</t>
-  </si>
-  <si>
-    <t>Hoffenheim,L L D W L W</t>
-  </si>
-  <si>
-    <t>Leverkusen,W L W W W L</t>
-  </si>
-  <si>
-    <t>Mainz,W W D L L L</t>
-  </si>
-  <si>
-    <t>Mgladbach,L W L W W D</t>
-  </si>
-  <si>
-    <t>RB Leipzig,L L D W W D</t>
-  </si>
-  <si>
-    <t>Stuttgart,L D L D W D</t>
-  </si>
-  <si>
-    <t>Union Berlin,W D L W W W</t>
-  </si>
-  <si>
-    <t>Wolfsburg,W W D L L L</t>
-  </si>
-  <si>
-    <t>Augsburg,1 0 1 0 1 1,(4)</t>
-  </si>
-  <si>
-    <t>Bayern Munich,5 4 7 3 1 5,(25)</t>
-  </si>
-  <si>
-    <t>Bielefeld,1 1 0 0 0 1,(3)</t>
-  </si>
-  <si>
-    <t>Bochum,1 1 0 0 0 1,(3)</t>
-  </si>
-  <si>
-    <t>Dortmund,3 4 4 0 2 3,(16)</t>
-  </si>
-  <si>
-    <t>Ein Frankfurt,1 1 1 1 2 1,(7)</t>
-  </si>
-  <si>
-    <t>FC Koln,2 1 1 1 3 0,(8)</t>
-  </si>
-  <si>
-    <t>Freiburg,3 1 0 3 2 1,(10)</t>
-  </si>
-  <si>
-    <t>Greuther Furth,0 0 1 1 1 0,(3)</t>
-  </si>
-  <si>
-    <t>Hertha,0 3 2 0 1 2,(8)</t>
-  </si>
-  <si>
-    <t>Hoffenheim,2 0 0 3 1 5,(11)</t>
-  </si>
-  <si>
-    <t>Leverkusen,4 3 3 1 4 1,(16)</t>
-  </si>
-  <si>
-    <t>Mainz,3 2 0 0 1 1,(7)</t>
-  </si>
-  <si>
-    <t>Mgladbach,1 3 0 1 3 1,(9)</t>
-  </si>
-  <si>
-    <t>RB Leipzig,0 1 1 6 3 1,(12)</t>
-  </si>
-  <si>
-    <t>Stuttgart,2 1 1 0 3 1,(8)</t>
-  </si>
-  <si>
-    <t>Union Berlin,2 0 2 1 2 2,(9)</t>
-  </si>
-  <si>
-    <t>Wolfsburg,1 2 1 1 1 0,(6)</t>
-  </si>
-  <si>
-    <t>Augsburg,4 0 0 3 2 1,(10)</t>
-  </si>
-  <si>
-    <t>Bayern Munich,0 1 0 1 2 1,(5)</t>
-  </si>
-  <si>
-    <t>Bielefeld,1 3 0 1 4 1,(10)</t>
-  </si>
-  <si>
-    <t>Bochum,2 3 7 0 3 0,(15)</t>
-  </si>
-  <si>
-    <t>Dortmund,2 3 2 1 1 1,(10)</t>
-  </si>
-  <si>
-    <t>Ein Frankfurt,1 1 1 1 1 2,(7)</t>
-  </si>
-  <si>
-    <t>FC Koln,1 1 1 1 1 5,(10)</t>
-  </si>
-  <si>
-    <t>Freiburg,2 1 0 0 1 1,(5)</t>
-  </si>
-  <si>
-    <t>Greuther Furth,3 2 2 3 3 1,(14)</t>
-  </si>
-  <si>
-    <t>Hertha,5 1 1 6 2 1,(16)</t>
-  </si>
-  <si>
-    <t>Hoffenheim,3 2 0 1 3 0,(9)</t>
-  </si>
-  <si>
-    <t>Leverkusen,1 4 1 0 0 5,(11)</t>
-  </si>
-  <si>
-    <t>Mainz,0 0 0 1 2 3,(6)</t>
-  </si>
-  <si>
-    <t>Mgladbach,2 1 1 0 1 1,(6)</t>
-  </si>
-  <si>
-    <t>RB Leipzig,1 4 1 0 0 1,(7)</t>
-  </si>
-  <si>
-    <t>Stuttgart,3 1 3 0 1 1,(9)</t>
-  </si>
-  <si>
-    <t>Union Berlin,1 0 4 0 1 0,(6)</t>
-  </si>
-  <si>
-    <t>Wolfsburg,0 0 1 3 3 2,(9)</t>
-  </si>
-  <si>
-    <t>Augsburg,5 0 1 3 3 2,(14)</t>
-  </si>
-  <si>
-    <t>Bayern Munich,5 5 7 4 3 6,(30)</t>
-  </si>
-  <si>
-    <t>Bielefeld,2 4 0 1 4 2,(13)</t>
-  </si>
-  <si>
-    <t>Bochum,3 4 7 0 3 1,(18)</t>
-  </si>
-  <si>
-    <t>Dortmund,5 7 6 1 3 4,(26)</t>
-  </si>
-  <si>
-    <t>Ein Frankfurt,2 2 2 2 3 3,(14)</t>
-  </si>
-  <si>
-    <t>FC Koln,3 2 2 2 4 5,(18)</t>
-  </si>
-  <si>
-    <t>Freiburg,5 2 0 3 3 2,(15)</t>
-  </si>
-  <si>
-    <t>Greuther Furth,3 2 3 4 4 1,(17)</t>
-  </si>
-  <si>
-    <t>Hertha,5 4 3 6 3 3,(24)</t>
-  </si>
-  <si>
-    <t>Hoffenheim,5 2 0 4 4 5,(20)</t>
-  </si>
-  <si>
-    <t>Leverkusen,5 7 4 1 4 6,(27)</t>
-  </si>
-  <si>
-    <t>Mainz,3 2 0 1 3 4,(13)</t>
-  </si>
-  <si>
-    <t>Mgladbach,3 4 1 1 4 2,(15)</t>
-  </si>
-  <si>
-    <t>RB Leipzig,1 5 2 6 3 2,(19)</t>
-  </si>
-  <si>
-    <t>Stuttgart,5 2 4 0 4 2,(17)</t>
-  </si>
-  <si>
-    <t>Union Berlin,3 0 6 1 3 2,(15)</t>
-  </si>
-  <si>
-    <t>Wolfsburg,1 2 2 4 4 2,(15)</t>
-  </si>
-  <si>
-    <t>Augsburg,1-4 0-0 1-0 3-0 2-1 1-1</t>
-  </si>
-  <si>
-    <t>Bayern Munich,5-0 1-4 7-0 1-3 1-2 1-5</t>
-  </si>
-  <si>
-    <t>Bielefeld,1-1 3-1 0-0 1-0 0-4 1-1</t>
-  </si>
-  <si>
-    <t>Bochum,2-1 1-3 7-0 0-0 3-0 0-1</t>
-  </si>
-  <si>
-    <t>Dortmund,3-2 3-4 4-2 1-0 2-1 3-1</t>
-  </si>
-  <si>
-    <t>Ein Frankfurt,1-1 1-1 1-1 1-1 1-2 1-2</t>
-  </si>
-  <si>
-    <t>FC Koln,2-1 1-1 1-1 1-1 3-1 5-0</t>
-  </si>
-  <si>
-    <t>Freiburg,2-3 1-1 0-0 3-0 1-2 1-1</t>
-  </si>
-  <si>
-    <t>Greuther Furth,3-0 0-2 2-1 1-3 3-1 0-1</t>
-  </si>
-  <si>
-    <t>Hertha,5-0 1-3 2-1 6-0 1-2 1-2</t>
-  </si>
-  <si>
-    <t>Hoffenheim,3-2 0-2 0-0 3-1 3-1 5-0</t>
-  </si>
-  <si>
-    <t>Leverkusen,1-4 3-4 1-3 1-0 0-4 1-5</t>
-  </si>
-  <si>
-    <t>Mainz,3-0 0-2 0-0 1-0 1-2 3-1</t>
-  </si>
-  <si>
-    <t>Mgladbach,2-1 3-1 1-0 1-0 1-3 1-1</t>
-  </si>
-  <si>
-    <t>RB Leipzig,1-0 1-4 1-1 6-0 3-0 1-1</t>
-  </si>
-  <si>
-    <t>Stuttgart,2-3 1-1 1-3 0-0 3-1 1-1</t>
-  </si>
-  <si>
-    <t>Union Berlin,2-1 0-0 4-2 1-0 1-2 2-0</t>
-  </si>
-  <si>
-    <t>Wolfsburg,1-0 0-2 1-1 3-1 1-3 2-0</t>
-  </si>
-  <si>
-    <t>Augsburg,-3 0 1 -3 -1 0,(-6)</t>
-  </si>
-  <si>
-    <t>Bayern Munich,5 3 7 2 -1 4,(20)</t>
-  </si>
-  <si>
-    <t>Bielefeld,0 -2 0 -1 -4 0,(-7)</t>
-  </si>
-  <si>
-    <t>Bochum,-1 -2 -7 0 -3 1,(-12)</t>
-  </si>
-  <si>
-    <t>Dortmund,1 1 2 -1 1 2,(6)</t>
-  </si>
-  <si>
-    <t>Ein Frankfurt,0 0 0 0 1 -1,(0)</t>
-  </si>
-  <si>
-    <t>FC Koln,1 0 0 0 2 -5,(-2)</t>
-  </si>
-  <si>
-    <t>Freiburg,1 0 0 3 1 0,(5)</t>
-  </si>
-  <si>
-    <t>Greuther Furth,-3 -2 -1 -2 -2 -1,(-11)</t>
-  </si>
-  <si>
-    <t>Hertha,-5 2 1 -6 -1 1,(-8)</t>
-  </si>
-  <si>
-    <t>Hoffenheim,-1 -2 0 2 -2 5,(2)</t>
-  </si>
-  <si>
-    <t>Leverkusen,3 -1 2 1 4 -4,(5)</t>
-  </si>
-  <si>
-    <t>Mainz,3 2 0 -1 -1 -2,(1)</t>
-  </si>
-  <si>
-    <t>Mgladbach,-1 2 -1 1 2 0,(3)</t>
-  </si>
-  <si>
-    <t>RB Leipzig,-1 -3 0 6 3 0,(5)</t>
-  </si>
-  <si>
-    <t>Stuttgart,-1 0 -2 0 2 0,(-1)</t>
-  </si>
-  <si>
-    <t>Union Berlin,1 0 -2 1 1 2,(3)</t>
-  </si>
-  <si>
-    <t>Wolfsburg,1 2 0 -2 -2 -2,(-3)</t>
-  </si>
-  <si>
-    <t>Augsburg,Leverkusen(4) Union Berlin(5) Mgladbach(9) Freiburg(3) Dortmund(2) Bielefeld(17)</t>
-  </si>
-  <si>
-    <t>Bayern Munich,Hertha(12) RB Leipzig(10) Bochum(15) Greuther Furth(18) Ein Frankfurt(14) Leverkusen(4)</t>
-  </si>
-  <si>
-    <t>Bielefeld,Ein Frankfurt(14) Mgladbach(9) Hoffenheim(8) Union Berlin(5) Leverkusen(4) Augsburg(16)</t>
-  </si>
-  <si>
-    <t>Bochum,FC Koln(7) Hertha(12) Bayern Munich(1) Stuttgart(13) RB Leipzig(10) Greuther Furth(18)</t>
-  </si>
-  <si>
-    <t>Dortmund,Hoffenheim(8) Leverkusen(4) Union Berlin(5) Mgladbach(9) Augsburg(16) Mainz(11)</t>
-  </si>
-  <si>
-    <t>Ein Frankfurt,Bielefeld(17) Stuttgart(13) Wolfsburg(6) FC Koln(7) Bayern Munich(1) Hertha(12)</t>
-  </si>
-  <si>
-    <t>FC Koln,Bochum(15) Freiburg(3) RB Leipzig(10) Ein Frankfurt(14) Greuther Furth(18) Hoffenheim(8)</t>
-  </si>
-  <si>
-    <t>Freiburg,Stuttgart(13) FC Koln(7) Mainz(11) Augsburg(16) Hertha(12) RB Leipzig(10)</t>
-  </si>
-  <si>
-    <t>Greuther Furth,Mainz(11) Wolfsburg(6) Hertha(12) Bayern Munich(1) FC Koln(7) Bochum(15)</t>
-  </si>
-  <si>
-    <t>Hertha,Bayern Munich(1) Bochum(15) Greuther Furth(18) RB Leipzig(10) Freiburg(3) Ein Frankfurt(14)</t>
-  </si>
-  <si>
-    <t>Hoffenheim,Dortmund(2) Mainz(11) Bielefeld(17) Wolfsburg(6) Stuttgart(13) FC Koln(7)</t>
-  </si>
-  <si>
-    <t>Leverkusen,Augsburg(16) Dortmund(2) Stuttgart(13) Mainz(11) Bielefeld(17) Bayern Munich(1)</t>
-  </si>
-  <si>
-    <t>Mainz,Greuther Furth(18) Hoffenheim(8) Freiburg(3) Leverkusen(4) Union Berlin(5) Dortmund(2)</t>
-  </si>
-  <si>
-    <t>Mgladbach,Union Berlin(5) Bielefeld(17) Augsburg(16) Dortmund(2) Wolfsburg(6) Stuttgart(13)</t>
-  </si>
-  <si>
-    <t>RB Leipzig,Wolfsburg(6) Bayern Munich(1) FC Koln(7) Hertha(12) Bochum(15) Freiburg(3)</t>
-  </si>
-  <si>
-    <t>Stuttgart,Freiburg(3) Ein Frankfurt(14) Leverkusen(4) Bochum(15) Hoffenheim(8) Mgladbach(9)</t>
-  </si>
-  <si>
-    <t>Union Berlin,Mgladbach(9) Augsburg(16) Dortmund(2) Bielefeld(17) Mainz(11) Wolfsburg(6)</t>
-  </si>
-  <si>
-    <t>Wolfsburg,RB Leipzig(10) Greuther Furth(18) Ein Frankfurt(14) Hoffenheim(8) Mgladbach(9) Union Berlin(5)</t>
+    <t>Augsburg,L D L D W L L D</t>
+  </si>
+  <si>
+    <t>Bayern Munich,D W W W W W L W</t>
+  </si>
+  <si>
+    <t>Bielefeld,D D D L D L L D</t>
+  </si>
+  <si>
+    <t>Bochum,L W L L L D L W</t>
+  </si>
+  <si>
+    <t>Dortmund,W L W W W L W W</t>
+  </si>
+  <si>
+    <t>Ein Frankfurt,L D D D D D W L</t>
+  </si>
+  <si>
+    <t>FC Koln,W L W D D D W L</t>
+  </si>
+  <si>
+    <t>Freiburg,D W W D D W W D</t>
+  </si>
+  <si>
+    <t>Greuther Furth,L D L L L L L L</t>
+  </si>
+  <si>
+    <t>Hertha,L L L W W L L W</t>
+  </si>
+  <si>
+    <t>Hoffenheim,W D L L D W L W</t>
+  </si>
+  <si>
+    <t>Leverkusen,D W W L W W W L</t>
+  </si>
+  <si>
+    <t>Mainz,W L W W D L L L</t>
+  </si>
+  <si>
+    <t>Mgladbach,D L L W L W W D</t>
+  </si>
+  <si>
+    <t>RB Leipzig,L W L L D W W D</t>
+  </si>
+  <si>
+    <t>Stuttgart,W L L D L D W D</t>
+  </si>
+  <si>
+    <t>Union Berlin,D D W D L W W W</t>
+  </si>
+  <si>
+    <t>Wolfsburg,W W W W D L L L</t>
+  </si>
+  <si>
+    <t>Augsburg,0 0 1 0 1 0 1 1,(4)</t>
+  </si>
+  <si>
+    <t>Bayern Munich,1 3 5 4 7 3 1 5,(29)</t>
+  </si>
+  <si>
+    <t>Bielefeld,0 1 1 1 0 0 0 1,(4)</t>
+  </si>
+  <si>
+    <t>Bochum,0 2 1 1 0 0 0 1,(5)</t>
+  </si>
+  <si>
+    <t>Dortmund,5 1 3 4 4 0 2 3,(22)</t>
+  </si>
+  <si>
+    <t>Ein Frankfurt,2 0 1 1 1 1 2 1,(9)</t>
+  </si>
+  <si>
+    <t>FC Koln,3 2 2 1 1 1 3 0,(13)</t>
+  </si>
+  <si>
+    <t>Freiburg,0 2 3 1 0 3 2 1,(12)</t>
+  </si>
+  <si>
+    <t>Greuther Furth,1 1 0 0 1 1 1 0,(5)</t>
+  </si>
+  <si>
+    <t>Hertha,1 1 0 3 2 0 1 2,(10)</t>
+  </si>
+  <si>
+    <t>Hoffenheim,4 2 2 0 0 3 1 5,(17)</t>
+  </si>
+  <si>
+    <t>Leverkusen,1 4 4 3 3 1 4 1,(21)</t>
+  </si>
+  <si>
+    <t>Mainz,1 0 3 2 0 0 1 1,(8)</t>
+  </si>
+  <si>
+    <t>Mgladbach,1 0 1 3 0 1 3 1,(10)</t>
+  </si>
+  <si>
+    <t>RB Leipzig,0 4 0 1 1 6 3 1,(16)</t>
+  </si>
+  <si>
+    <t>Stuttgart,5 0 2 1 1 0 3 1,(13)</t>
+  </si>
+  <si>
+    <t>Union Berlin,1 2 2 0 2 1 2 2,(12)</t>
+  </si>
+  <si>
+    <t>Wolfsburg,1 2 1 2 1 1 1 0,(9)</t>
+  </si>
+  <si>
+    <t>Augsburg,4 0 4 0 0 3 2 1,(14)</t>
+  </si>
+  <si>
+    <t>Bayern Munich,1 2 0 1 0 1 2 1,(8)</t>
+  </si>
+  <si>
+    <t>Bielefeld,0 1 1 3 0 1 4 1,(11)</t>
+  </si>
+  <si>
+    <t>Bochum,1 0 2 3 7 0 3 0,(16)</t>
+  </si>
+  <si>
+    <t>Dortmund,2 2 2 3 2 1 1 1,(14)</t>
+  </si>
+  <si>
+    <t>Ein Frankfurt,5 0 1 1 1 1 1 2,(12)</t>
+  </si>
+  <si>
+    <t>FC Koln,1 3 1 1 1 1 1 5,(14)</t>
+  </si>
+  <si>
+    <t>Freiburg,0 1 2 1 0 0 1 1,(6)</t>
+  </si>
+  <si>
+    <t>Greuther Furth,5 1 3 2 2 3 3 1,(20)</t>
+  </si>
+  <si>
+    <t>Hertha,3 2 5 1 1 6 2 1,(21)</t>
+  </si>
+  <si>
+    <t>Hoffenheim,0 2 3 2 0 1 3 0,(11)</t>
+  </si>
+  <si>
+    <t>Leverkusen,1 0 1 4 1 0 0 5,(12)</t>
+  </si>
+  <si>
+    <t>Mainz,0 2 0 0 0 1 2 3,(8)</t>
+  </si>
+  <si>
+    <t>Mgladbach,1 4 2 1 1 0 1 1,(11)</t>
+  </si>
+  <si>
+    <t>RB Leipzig,1 0 1 4 1 0 0 1,(8)</t>
+  </si>
+  <si>
+    <t>Stuttgart,1 4 3 1 3 0 1 1,(14)</t>
+  </si>
+  <si>
+    <t>Union Berlin,1 2 1 0 4 0 1 0,(9)</t>
+  </si>
+  <si>
+    <t>Wolfsburg,0 1 0 0 1 3 3 2,(10)</t>
+  </si>
+  <si>
+    <t>Augsburg,4 0 5 0 1 3 3 2,(18)</t>
+  </si>
+  <si>
+    <t>Bayern Munich,2 5 5 5 7 4 3 6,(37)</t>
+  </si>
+  <si>
+    <t>Bielefeld,0 2 2 4 0 1 4 2,(15)</t>
+  </si>
+  <si>
+    <t>Bochum,1 2 3 4 7 0 3 1,(21)</t>
+  </si>
+  <si>
+    <t>Dortmund,7 3 5 7 6 1 3 4,(36)</t>
+  </si>
+  <si>
+    <t>Ein Frankfurt,7 0 2 2 2 2 3 3,(21)</t>
+  </si>
+  <si>
+    <t>FC Koln,4 5 3 2 2 2 4 5,(27)</t>
+  </si>
+  <si>
+    <t>Freiburg,0 3 5 2 0 3 3 2,(18)</t>
+  </si>
+  <si>
+    <t>Greuther Furth,6 2 3 2 3 4 4 1,(25)</t>
+  </si>
+  <si>
+    <t>Hertha,4 3 5 4 3 6 3 3,(31)</t>
+  </si>
+  <si>
+    <t>Hoffenheim,4 4 5 2 0 4 4 5,(28)</t>
+  </si>
+  <si>
+    <t>Leverkusen,2 4 5 7 4 1 4 6,(33)</t>
+  </si>
+  <si>
+    <t>Mainz,1 2 3 2 0 1 3 4,(16)</t>
+  </si>
+  <si>
+    <t>Mgladbach,2 4 3 4 1 1 4 2,(21)</t>
+  </si>
+  <si>
+    <t>RB Leipzig,1 4 1 5 2 6 3 2,(24)</t>
+  </si>
+  <si>
+    <t>Stuttgart,6 4 5 2 4 0 4 2,(27)</t>
+  </si>
+  <si>
+    <t>Union Berlin,2 4 3 0 6 1 3 2,(21)</t>
+  </si>
+  <si>
+    <t>Wolfsburg,1 3 1 2 2 4 4 2,(19)</t>
+  </si>
+  <si>
+    <t>Augsburg,0-4 0-0 1-4 0-0 1-0 3-0 2-1 1-1</t>
+  </si>
+  <si>
+    <t>Bayern Munich,1-1 3-2 5-0 1-4 7-0 1-3 1-2 1-5</t>
+  </si>
+  <si>
+    <t>Bielefeld,0-0 1-1 1-1 3-1 0-0 1-0 0-4 1-1</t>
+  </si>
+  <si>
+    <t>Bochum,1-0 2-0 2-1 1-3 7-0 0-0 3-0 0-1</t>
+  </si>
+  <si>
+    <t>Dortmund,5-2 2-1 3-2 3-4 4-2 1-0 2-1 3-1</t>
+  </si>
+  <si>
+    <t>Ein Frankfurt,5-2 0-0 1-1 1-1 1-1 1-1 1-2 1-2</t>
+  </si>
+  <si>
+    <t>FC Koln,3-1 3-2 2-1 1-1 1-1 1-1 3-1 5-0</t>
+  </si>
+  <si>
+    <t>Freiburg,0-0 2-1 2-3 1-1 0-0 3-0 1-2 1-1</t>
+  </si>
+  <si>
+    <t>Greuther Furth,5-1 1-1 3-0 0-2 2-1 1-3 3-1 0-1</t>
+  </si>
+  <si>
+    <t>Hertha,3-1 1-2 5-0 1-3 2-1 6-0 1-2 1-2</t>
+  </si>
+  <si>
+    <t>Hoffenheim,0-4 2-2 3-2 0-2 0-0 3-1 3-1 5-0</t>
+  </si>
+  <si>
+    <t>Leverkusen,1-1 4-0 1-4 3-4 1-3 1-0 0-4 1-5</t>
+  </si>
+  <si>
+    <t>Mainz,1-0 2-0 3-0 0-2 0-0 1-0 1-2 3-1</t>
+  </si>
+  <si>
+    <t>Mgladbach,1-1 4-0 2-1 3-1 1-0 1-0 1-3 1-1</t>
+  </si>
+  <si>
+    <t>RB Leipzig,1-0 4-0 1-0 1-4 1-1 6-0 3-0 1-1</t>
+  </si>
+  <si>
+    <t>Stuttgart,5-1 4-0 2-3 1-1 1-3 0-0 3-1 1-1</t>
+  </si>
+  <si>
+    <t>Union Berlin,1-1 2-2 2-1 0-0 4-2 1-0 1-2 2-0</t>
+  </si>
+  <si>
+    <t>Wolfsburg,1-0 1-2 1-0 0-2 1-1 3-1 1-3 2-0</t>
+  </si>
+  <si>
+    <t>Augsburg,-4 0 -3 0 1 -3 -1 0,(-10)</t>
+  </si>
+  <si>
+    <t>Bayern Munich,0 1 5 3 7 2 -1 4,(21)</t>
+  </si>
+  <si>
+    <t>Bielefeld,0 0 0 -2 0 -1 -4 0,(-7)</t>
+  </si>
+  <si>
+    <t>Bochum,-1 2 -1 -2 -7 0 -3 1,(-11)</t>
+  </si>
+  <si>
+    <t>Dortmund,3 -1 1 1 2 -1 1 2,(8)</t>
+  </si>
+  <si>
+    <t>Ein Frankfurt,-3 0 0 0 0 0 1 -1,(-3)</t>
+  </si>
+  <si>
+    <t>FC Koln,2 -1 1 0 0 0 2 -5,(-1)</t>
+  </si>
+  <si>
+    <t>Freiburg,0 1 1 0 0 3 1 0,(6)</t>
+  </si>
+  <si>
+    <t>Greuther Furth,-4 0 -3 -2 -1 -2 -2 -1,(-15)</t>
+  </si>
+  <si>
+    <t>Hertha,-2 -1 -5 2 1 -6 -1 1,(-11)</t>
+  </si>
+  <si>
+    <t>Hoffenheim,4 0 -1 -2 0 2 -2 5,(6)</t>
+  </si>
+  <si>
+    <t>Leverkusen,0 4 3 -1 2 1 4 -4,(9)</t>
+  </si>
+  <si>
+    <t>Mainz,1 -2 3 2 0 -1 -1 -2,(0)</t>
+  </si>
+  <si>
+    <t>Mgladbach,0 -4 -1 2 -1 1 2 0,(-1)</t>
+  </si>
+  <si>
+    <t>RB Leipzig,-1 4 -1 -3 0 6 3 0,(8)</t>
+  </si>
+  <si>
+    <t>Stuttgart,4 -4 -1 0 -2 0 2 0,(-1)</t>
+  </si>
+  <si>
+    <t>Union Berlin,0 0 1 0 -2 1 1 2,(3)</t>
+  </si>
+  <si>
+    <t>Wolfsburg,1 1 1 2 0 -2 -2 -2,(-1)</t>
+  </si>
+  <si>
+    <t>Augsburg,Hoffenheim(8) Ein Frankfurt(14) Leverkusen(4) Union Berlin(5) Mgladbach(9) Freiburg(3) Dortmund(2) Bielefeld(17)</t>
+  </si>
+  <si>
+    <t>Bayern Munich,Mgladbach(9) FC Koln(7) Hertha(12) RB Leipzig(10) Bochum(15) Greuther Furth(18) Ein Frankfurt(14) Leverkusen(4)</t>
+  </si>
+  <si>
+    <t>Bielefeld,Freiburg(3) Greuther Furth(18) Ein Frankfurt(14) Mgladbach(9) Hoffenheim(8) Union Berlin(5) Leverkusen(4) Augsburg(16)</t>
+  </si>
+  <si>
+    <t>Bochum,Wolfsburg(6) Mainz(11) FC Koln(7) Hertha(12) Bayern Munich(1) Stuttgart(13) RB Leipzig(10) Greuther Furth(18)</t>
+  </si>
+  <si>
+    <t>Dortmund,Ein Frankfurt(14) Freiburg(3) Hoffenheim(8) Leverkusen(4) Union Berlin(5) Mgladbach(9) Augsburg(16) Mainz(11)</t>
+  </si>
+  <si>
+    <t>Ein Frankfurt,Dortmund(2) Augsburg(16) Bielefeld(17) Stuttgart(13) Wolfsburg(6) FC Koln(7) Bayern Munich(1) Hertha(12)</t>
+  </si>
+  <si>
+    <t>FC Koln,Hertha(12) Bayern Munich(1) Bochum(15) Freiburg(3) RB Leipzig(10) Ein Frankfurt(14) Greuther Furth(18) Hoffenheim(8)</t>
+  </si>
+  <si>
+    <t>Freiburg,Bielefeld(17) Dortmund(2) Stuttgart(13) FC Koln(7) Mainz(11) Augsburg(16) Hertha(12) RB Leipzig(10)</t>
+  </si>
+  <si>
+    <t>Greuther Furth,Stuttgart(13) Bielefeld(17) Mainz(11) Wolfsburg(6) Hertha(12) Bayern Munich(1) FC Koln(7) Bochum(15)</t>
+  </si>
+  <si>
+    <t>Hertha,FC Koln(7) Wolfsburg(6) Bayern Munich(1) Bochum(15) Greuther Furth(18) RB Leipzig(10) Freiburg(3) Ein Frankfurt(14)</t>
+  </si>
+  <si>
+    <t>Hoffenheim,Augsburg(16) Union Berlin(5) Dortmund(2) Mainz(11) Bielefeld(17) Wolfsburg(6) Stuttgart(13) FC Koln(7)</t>
+  </si>
+  <si>
+    <t>Leverkusen,Union Berlin(5) Mgladbach(9) Augsburg(16) Dortmund(2) Stuttgart(13) Mainz(11) Bielefeld(17) Bayern Munich(1)</t>
+  </si>
+  <si>
+    <t>Mainz,RB Leipzig(10) Bochum(15) Greuther Furth(18) Hoffenheim(8) Freiburg(3) Leverkusen(4) Union Berlin(5) Dortmund(2)</t>
+  </si>
+  <si>
+    <t>Mgladbach,Bayern Munich(1) Leverkusen(4) Union Berlin(5) Bielefeld(17) Augsburg(16) Dortmund(2) Wolfsburg(6) Stuttgart(13)</t>
+  </si>
+  <si>
+    <t>RB Leipzig,Mainz(11) Stuttgart(13) Wolfsburg(6) Bayern Munich(1) FC Koln(7) Hertha(12) Bochum(15) Freiburg(3)</t>
+  </si>
+  <si>
+    <t>Stuttgart,Greuther Furth(18) RB Leipzig(10) Freiburg(3) Ein Frankfurt(14) Leverkusen(4) Bochum(15) Hoffenheim(8) Mgladbach(9)</t>
+  </si>
+  <si>
+    <t>Union Berlin,Leverkusen(4) Hoffenheim(8) Mgladbach(9) Augsburg(16) Dortmund(2) Bielefeld(17) Mainz(11) Wolfsburg(6)</t>
+  </si>
+  <si>
+    <t>Wolfsburg,Bochum(15) Hertha(12) RB Leipzig(10) Greuther Furth(18) Ein Frankfurt(14) Hoffenheim(8) Mgladbach(9) Union Berlin(5)</t>
   </si>
   <si>
     <t>Div</t>

</xml_diff>

<commit_message>
updated error in masterwrit
</commit_message>
<xml_diff>
--- a/Divisions/D1.xlsx
+++ b/Divisions/D1.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9655" uniqueCount="1711">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9677" uniqueCount="1711">
   <si>
     <t>Team</t>
   </si>
@@ -95052,6 +95052,15 @@
       <c r="V1" t="s">
         <v>105</v>
       </c>
+      <c r="W1" t="s">
+        <v>106</v>
+      </c>
+      <c r="X1" t="s">
+        <v>107</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
@@ -95120,6 +95129,15 @@
       <c r="V2" t="s">
         <v>4</v>
       </c>
+      <c r="W2" t="s">
+        <v>2</v>
+      </c>
+      <c r="X2" t="s">
+        <v>4</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
@@ -95188,6 +95206,15 @@
       <c r="V3" t="s">
         <v>2</v>
       </c>
+      <c r="W3" t="s">
+        <v>2</v>
+      </c>
+      <c r="X3" t="s">
+        <v>4</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
@@ -95256,6 +95283,15 @@
       <c r="V4" t="s">
         <v>2</v>
       </c>
+      <c r="W4" t="s">
+        <v>3</v>
+      </c>
+      <c r="X4" t="s">
+        <v>4</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
@@ -95324,6 +95360,15 @@
       <c r="V5" t="s">
         <v>3</v>
       </c>
+      <c r="W5" t="s">
+        <v>3</v>
+      </c>
+      <c r="X5" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
@@ -95392,6 +95437,15 @@
       <c r="V6" t="s">
         <v>2</v>
       </c>
+      <c r="W6" t="s">
+        <v>4</v>
+      </c>
+      <c r="X6" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y6" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
@@ -95460,6 +95514,15 @@
       <c r="V7" t="s">
         <v>4</v>
       </c>
+      <c r="W7" t="s">
+        <v>2</v>
+      </c>
+      <c r="X7" t="s">
+        <v>4</v>
+      </c>
+      <c r="Y7" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
@@ -95528,6 +95591,15 @@
       <c r="V8" t="s">
         <v>3</v>
       </c>
+      <c r="W8" t="s">
+        <v>2</v>
+      </c>
+      <c r="X8" t="s">
+        <v>4</v>
+      </c>
+      <c r="Y8" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
@@ -95596,6 +95668,15 @@
       <c r="V9" t="s">
         <v>2</v>
       </c>
+      <c r="W9" t="s">
+        <v>4</v>
+      </c>
+      <c r="X9" t="s">
+        <v>3</v>
+      </c>
+      <c r="Y9" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
@@ -95664,6 +95745,15 @@
       <c r="V10" t="s">
         <v>2</v>
       </c>
+      <c r="W10" t="s">
+        <v>4</v>
+      </c>
+      <c r="X10" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y10" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
@@ -95732,6 +95822,15 @@
       <c r="V11" t="s">
         <v>4</v>
       </c>
+      <c r="W11" t="s">
+        <v>3</v>
+      </c>
+      <c r="X11" t="s">
+        <v>4</v>
+      </c>
+      <c r="Y11" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
@@ -95800,6 +95899,15 @@
       <c r="V12" t="s">
         <v>4</v>
       </c>
+      <c r="W12" t="s">
+        <v>4</v>
+      </c>
+      <c r="X12" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y12" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
@@ -95868,6 +95976,15 @@
       <c r="V13" t="s">
         <v>2</v>
       </c>
+      <c r="W13" t="s">
+        <v>2</v>
+      </c>
+      <c r="X13" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y13" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
@@ -95936,6 +96053,15 @@
       <c r="V14" t="s">
         <v>4</v>
       </c>
+      <c r="W14" t="s">
+        <v>2</v>
+      </c>
+      <c r="X14" t="s">
+        <v>3</v>
+      </c>
+      <c r="Y14" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
@@ -96004,6 +96130,15 @@
       <c r="V15" t="s">
         <v>4</v>
       </c>
+      <c r="W15" t="s">
+        <v>3</v>
+      </c>
+      <c r="X15" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y15" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
@@ -96072,6 +96207,15 @@
       <c r="V16" t="s">
         <v>2</v>
       </c>
+      <c r="W16" t="s">
+        <v>4</v>
+      </c>
+      <c r="X16" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y16" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
@@ -96140,6 +96284,15 @@
       <c r="V17" t="s">
         <v>4</v>
       </c>
+      <c r="W17" t="s">
+        <v>4</v>
+      </c>
+      <c r="X17" t="s">
+        <v>4</v>
+      </c>
+      <c r="Y17" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
@@ -96208,6 +96361,15 @@
       <c r="V18" t="s">
         <v>2</v>
       </c>
+      <c r="W18" t="s">
+        <v>4</v>
+      </c>
+      <c r="X18" t="s">
+        <v>4</v>
+      </c>
+      <c r="Y18" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
@@ -96274,6 +96436,15 @@
         <v>3</v>
       </c>
       <c r="V19" t="s">
+        <v>4</v>
+      </c>
+      <c r="W19" t="s">
+        <v>2</v>
+      </c>
+      <c r="X19" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y19" t="s">
         <v>4</v>
       </c>
     </row>
@@ -96296,75 +96467,72 @@
         <v>85</v>
       </c>
       <c r="C1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="E1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="F1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="G1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="H1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="I1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="J1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="K1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="L1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="M1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="N1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="O1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="P1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="Q1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="R1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="S1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="T1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="U1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="V1" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="W1" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="X1" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="Y1" t="s">
-        <v>107</v>
-      </c>
-      <c r="Z1" t="s">
         <v>108</v>
       </c>
     </row>
@@ -96375,26 +96543,26 @@
       <c r="B2" t="s">
         <v>43</v>
       </c>
-      <c r="C2" t="s">
-        <v>43</v>
+      <c r="C2" t="n">
+        <v>0.0</v>
       </c>
       <c r="D2" t="n">
         <v>0.0</v>
       </c>
       <c r="E2" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="F2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G2" t="n">
         <v>1.0</v>
       </c>
-      <c r="G2" t="n">
-        <v>0.0</v>
-      </c>
       <c r="H2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I2" t="n">
         <v>1.0</v>
-      </c>
-      <c r="I2" t="n">
-        <v>0.0</v>
       </c>
       <c r="J2" t="n">
         <v>1.0</v>
@@ -96403,31 +96571,31 @@
         <v>1.0</v>
       </c>
       <c r="L2" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="M2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="N2" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="O2" t="n">
         <v>1.0</v>
       </c>
-      <c r="M2" t="n">
-        <v>4.0</v>
-      </c>
-      <c r="N2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="O2" t="n">
+      <c r="P2" t="n">
         <v>2.0</v>
-      </c>
-      <c r="P2" t="n">
-        <v>1.0</v>
       </c>
       <c r="Q2" t="n">
         <v>2.0</v>
       </c>
       <c r="R2" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="S2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="T2" t="n">
         <v>1.0</v>
-      </c>
-      <c r="T2" t="n">
-        <v>0.0</v>
       </c>
       <c r="U2" t="n">
         <v>1.0</v>
@@ -96436,15 +96604,12 @@
         <v>1.0</v>
       </c>
       <c r="W2" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="X2" t="n">
         <v>2.0</v>
       </c>
       <c r="Y2" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="Z2" t="n">
         <v>1.0</v>
       </c>
     </row>
@@ -96455,76 +96620,73 @@
       <c r="B3" t="s">
         <v>28</v>
       </c>
-      <c r="C3" t="s">
-        <v>28</v>
+      <c r="C3" t="n">
+        <v>1.0</v>
       </c>
       <c r="D3" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="E3" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="F3" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="G3" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="H3" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="I3" t="n">
         <v>1.0</v>
       </c>
-      <c r="E3" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="F3" t="n">
+      <c r="J3" t="n">
         <v>5.0</v>
       </c>
-      <c r="G3" t="n">
+      <c r="K3" t="n">
         <v>4.0</v>
       </c>
-      <c r="H3" t="n">
-        <v>7.0</v>
-      </c>
-      <c r="I3" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="J3" t="n">
+      <c r="L3" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="M3" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="N3" t="n">
         <v>1.0</v>
-      </c>
-      <c r="K3" t="n">
-        <v>5.0</v>
-      </c>
-      <c r="L3" t="n">
-        <v>4.0</v>
-      </c>
-      <c r="M3" t="n">
-        <v>5.0</v>
-      </c>
-      <c r="N3" t="n">
-        <v>2.0</v>
       </c>
       <c r="O3" t="n">
         <v>1.0</v>
       </c>
       <c r="P3" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="R3" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="S3" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="T3" t="n">
         <v>1.0</v>
       </c>
-      <c r="Q3" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="R3" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="S3" t="n">
-        <v>5.0</v>
-      </c>
-      <c r="T3" t="n">
+      <c r="U3" t="n">
         <v>4.0</v>
-      </c>
-      <c r="U3" t="n">
-        <v>1.0</v>
       </c>
       <c r="V3" t="n">
         <v>4.0</v>
       </c>
       <c r="W3" t="n">
-        <v>4.0</v>
+        <v>3.0</v>
       </c>
       <c r="X3" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="Y3" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="Z3" t="n">
         <v>4.0</v>
       </c>
     </row>
@@ -96535,11 +96697,11 @@
       <c r="B4" t="s">
         <v>41</v>
       </c>
-      <c r="C4" t="s">
-        <v>41</v>
+      <c r="C4" t="n">
+        <v>0.0</v>
       </c>
       <c r="D4" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="E4" t="n">
         <v>1.0</v>
@@ -96548,16 +96710,16 @@
         <v>1.0</v>
       </c>
       <c r="G4" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="J4" t="n">
         <v>1.0</v>
-      </c>
-      <c r="H4" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="I4" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="J4" t="n">
-        <v>0.0</v>
       </c>
       <c r="K4" t="n">
         <v>1.0</v>
@@ -96569,19 +96731,19 @@
         <v>1.0</v>
       </c>
       <c r="N4" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="O4" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="P4" t="n">
         <v>1.0</v>
       </c>
-      <c r="O4" t="n">
+      <c r="Q4" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="R4" t="n">
         <v>2.0</v>
-      </c>
-      <c r="P4" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="Q4" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="R4" t="n">
-        <v>0.0</v>
       </c>
       <c r="S4" t="n">
         <v>2.0</v>
@@ -96596,15 +96758,12 @@
         <v>2.0</v>
       </c>
       <c r="W4" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="X4" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="Y4" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="Z4" t="n">
         <v>1.0</v>
       </c>
     </row>
@@ -96615,76 +96774,73 @@
       <c r="B5" t="s">
         <v>38</v>
       </c>
-      <c r="C5" t="s">
-        <v>38</v>
+      <c r="C5" t="n">
+        <v>0.0</v>
       </c>
       <c r="D5" t="n">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
       <c r="E5" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="F5" t="n">
         <v>1.0</v>
       </c>
       <c r="G5" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="J5" t="n">
         <v>1.0</v>
       </c>
-      <c r="H5" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="I5" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="J5" t="n">
-        <v>0.0</v>
-      </c>
       <c r="K5" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="L5" t="n">
         <v>1.0</v>
       </c>
-      <c r="L5" t="n">
+      <c r="M5" t="n">
         <v>2.0</v>
       </c>
-      <c r="M5" t="n">
+      <c r="N5" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="O5" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="P5" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="Q5" t="n">
         <v>1.0</v>
       </c>
-      <c r="N5" t="n">
+      <c r="R5" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="S5" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="T5" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="U5" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="V5" t="n">
         <v>2.0</v>
       </c>
-      <c r="O5" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="P5" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="Q5" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="R5" t="n">
+      <c r="W5" t="n">
         <v>1.0</v>
       </c>
-      <c r="S5" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="T5" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="U5" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="V5" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="W5" t="n">
-        <v>2.0</v>
-      </c>
       <c r="X5" t="n">
-        <v>1.0</v>
+        <v>4.0</v>
       </c>
       <c r="Y5" t="n">
-        <v>4.0</v>
-      </c>
-      <c r="Z5" t="n">
         <v>1.0</v>
       </c>
     </row>
@@ -96695,76 +96851,73 @@
       <c r="B6" t="s">
         <v>29</v>
       </c>
-      <c r="C6" t="s">
-        <v>29</v>
+      <c r="C6" t="n">
+        <v>5.0</v>
       </c>
       <c r="D6" t="n">
-        <v>5.0</v>
+        <v>1.0</v>
       </c>
       <c r="E6" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="F6" t="n">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
       <c r="G6" t="n">
         <v>4.0</v>
       </c>
       <c r="H6" t="n">
-        <v>4.0</v>
+        <v>0.0</v>
       </c>
       <c r="I6" t="n">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
       <c r="J6" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="K6" t="n">
         <v>3.0</v>
       </c>
       <c r="L6" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="M6" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="N6" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="O6" t="n">
         <v>3.0</v>
       </c>
-      <c r="M6" t="n">
+      <c r="P6" t="n">
         <v>2.0</v>
       </c>
-      <c r="N6" t="n">
+      <c r="Q6" t="n">
         <v>1.0</v>
       </c>
-      <c r="O6" t="n">
+      <c r="R6" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="S6" t="n">
         <v>2.0</v>
       </c>
-      <c r="P6" t="n">
+      <c r="T6" t="n">
         <v>3.0</v>
       </c>
-      <c r="Q6" t="n">
+      <c r="U6" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="V6" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="W6" t="n">
         <v>2.0</v>
       </c>
-      <c r="R6" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="S6" t="n">
+      <c r="X6" t="n">
         <v>3.0</v>
       </c>
-      <c r="T6" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="U6" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="V6" t="n">
-        <v>5.0</v>
-      </c>
-      <c r="W6" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="X6" t="n">
-        <v>2.0</v>
-      </c>
       <c r="Y6" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="Z6" t="n">
         <v>6.0</v>
       </c>
     </row>
@@ -96775,14 +96928,14 @@
       <c r="B7" t="s">
         <v>37</v>
       </c>
-      <c r="C7" t="s">
-        <v>37</v>
+      <c r="C7" t="n">
+        <v>2.0</v>
       </c>
       <c r="D7" t="n">
-        <v>2.0</v>
+        <v>0.0</v>
       </c>
       <c r="E7" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="F7" t="n">
         <v>1.0</v>
@@ -96794,19 +96947,19 @@
         <v>1.0</v>
       </c>
       <c r="I7" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="J7" t="n">
         <v>1.0</v>
       </c>
-      <c r="J7" t="n">
+      <c r="K7" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L7" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="M7" t="n">
         <v>2.0</v>
-      </c>
-      <c r="K7" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="L7" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="M7" t="n">
-        <v>1.0</v>
       </c>
       <c r="N7" t="n">
         <v>2.0</v>
@@ -96818,33 +96971,30 @@
         <v>2.0</v>
       </c>
       <c r="Q7" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="R7" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="S7" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="T7" t="n">
         <v>2.0</v>
       </c>
-      <c r="R7" t="n">
-        <v>5.0</v>
-      </c>
-      <c r="S7" t="n">
+      <c r="U7" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="V7" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="W7" t="n">
         <v>3.0</v>
       </c>
-      <c r="T7" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="U7" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="V7" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="W7" t="n">
-        <v>0.0</v>
-      </c>
       <c r="X7" t="n">
-        <v>3.0</v>
+        <v>0.0</v>
       </c>
       <c r="Y7" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="Z7" t="n">
         <v>0.0</v>
       </c>
     </row>
@@ -96855,17 +97005,17 @@
       <c r="B8" t="s">
         <v>34</v>
       </c>
-      <c r="C8" t="s">
-        <v>34</v>
+      <c r="C8" t="n">
+        <v>3.0</v>
       </c>
       <c r="D8" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="E8" t="n">
         <v>2.0</v>
       </c>
       <c r="F8" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="G8" t="n">
         <v>1.0</v>
@@ -96874,57 +97024,54 @@
         <v>1.0</v>
       </c>
       <c r="I8" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="J8" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K8" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="L8" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M8" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="N8" t="n">
         <v>1.0</v>
       </c>
-      <c r="J8" t="n">
+      <c r="O8" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="P8" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="R8" t="n">
         <v>3.0</v>
       </c>
-      <c r="K8" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="L8" t="n">
+      <c r="S8" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="T8" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="U8" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="V8" t="n">
         <v>2.0</v>
       </c>
-      <c r="M8" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="N8" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="O8" t="n">
+      <c r="W8" t="n">
         <v>1.0</v>
-      </c>
-      <c r="P8" t="n">
-        <v>4.0</v>
-      </c>
-      <c r="Q8" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="R8" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="S8" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="T8" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="U8" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="V8" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="W8" t="n">
-        <v>2.0</v>
       </c>
       <c r="X8" t="n">
         <v>1.0</v>
       </c>
       <c r="Y8" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="Z8" t="n">
         <v>1.0</v>
       </c>
     </row>
@@ -96935,76 +97082,73 @@
       <c r="B9" t="s">
         <v>31</v>
       </c>
-      <c r="C9" t="s">
-        <v>31</v>
+      <c r="C9" t="n">
+        <v>0.0</v>
       </c>
       <c r="D9" t="n">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
       <c r="E9" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F9" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H9" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="I9" t="n">
         <v>2.0</v>
       </c>
-      <c r="F9" t="n">
+      <c r="J9" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="K9" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="L9" t="n">
         <v>3.0</v>
       </c>
-      <c r="G9" t="n">
+      <c r="M9" t="n">
         <v>1.0</v>
       </c>
-      <c r="H9" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="I9" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="J9" t="n">
+      <c r="N9" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="O9" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="P9" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="R9" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="S9" t="n">
         <v>2.0</v>
-      </c>
-      <c r="K9" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="L9" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="M9" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="N9" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="O9" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="P9" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="Q9" t="n">
-        <v>6.0</v>
-      </c>
-      <c r="R9" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="S9" t="n">
-        <v>0.0</v>
       </c>
       <c r="T9" t="n">
         <v>2.0</v>
       </c>
       <c r="U9" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="V9" t="n">
         <v>2.0</v>
       </c>
-      <c r="V9" t="n">
+      <c r="W9" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X9" t="n">
         <v>1.0</v>
       </c>
-      <c r="W9" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="X9" t="n">
-        <v>0.0</v>
-      </c>
       <c r="Y9" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="Z9" t="n">
         <v>2.0</v>
       </c>
     </row>
@@ -97015,20 +97159,20 @@
       <c r="B10" t="s">
         <v>45</v>
       </c>
-      <c r="C10" t="s">
-        <v>45</v>
+      <c r="C10" t="n">
+        <v>1.0</v>
       </c>
       <c r="D10" t="n">
         <v>1.0</v>
       </c>
       <c r="E10" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G10" t="n">
         <v>1.0</v>
-      </c>
-      <c r="F10" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="G10" t="n">
-        <v>0.0</v>
       </c>
       <c r="H10" t="n">
         <v>1.0</v>
@@ -97037,10 +97181,10 @@
         <v>1.0</v>
       </c>
       <c r="J10" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K10" t="n">
         <v>1.0</v>
-      </c>
-      <c r="K10" t="n">
-        <v>0.0</v>
       </c>
       <c r="L10" t="n">
         <v>1.0</v>
@@ -97049,19 +97193,19 @@
         <v>1.0</v>
       </c>
       <c r="N10" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="O10" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="P10" t="n">
         <v>1.0</v>
-      </c>
-      <c r="O10" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="P10" t="n">
-        <v>3.0</v>
       </c>
       <c r="Q10" t="n">
         <v>1.0</v>
       </c>
       <c r="R10" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="S10" t="n">
         <v>0.0</v>
@@ -97070,21 +97214,18 @@
         <v>0.0</v>
       </c>
       <c r="U10" t="n">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
       <c r="V10" t="n">
         <v>2.0</v>
       </c>
       <c r="W10" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="X10" t="n">
         <v>2.0</v>
       </c>
-      <c r="X10" t="n">
-        <v>1.0</v>
-      </c>
       <c r="Y10" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="Z10" t="n">
         <v>1.0</v>
       </c>
     </row>
@@ -97095,65 +97236,65 @@
       <c r="B11" t="s">
         <v>42</v>
       </c>
-      <c r="C11" t="s">
-        <v>42</v>
+      <c r="C11" t="n">
+        <v>1.0</v>
       </c>
       <c r="D11" t="n">
         <v>1.0</v>
       </c>
       <c r="E11" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F11" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="G11" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="H11" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I11" t="n">
         <v>1.0</v>
       </c>
-      <c r="F11" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="G11" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="H11" t="n">
+      <c r="J11" t="n">
         <v>2.0</v>
       </c>
-      <c r="I11" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="J11" t="n">
+      <c r="K11" t="n">
         <v>1.0</v>
       </c>
-      <c r="K11" t="n">
+      <c r="L11" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M11" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="N11" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="O11" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="P11" t="n">
         <v>2.0</v>
-      </c>
-      <c r="L11" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="M11" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="N11" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="O11" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="P11" t="n">
-        <v>1.0</v>
       </c>
       <c r="Q11" t="n">
         <v>2.0</v>
       </c>
       <c r="R11" t="n">
-        <v>2.0</v>
+        <v>0.0</v>
       </c>
       <c r="S11" t="n">
-        <v>0.0</v>
+        <v>3.0</v>
       </c>
       <c r="T11" t="n">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
       <c r="U11" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="V11" t="n">
         <v>1.0</v>
-      </c>
-      <c r="V11" t="n">
-        <v>0.0</v>
       </c>
       <c r="W11" t="n">
         <v>1.0</v>
@@ -97162,9 +97303,6 @@
         <v>1.0</v>
       </c>
       <c r="Y11" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="Z11" t="n">
         <v>1.0</v>
       </c>
     </row>
@@ -97175,76 +97313,73 @@
       <c r="B12" t="s">
         <v>32</v>
       </c>
-      <c r="C12" t="s">
-        <v>32</v>
+      <c r="C12" t="n">
+        <v>4.0</v>
       </c>
       <c r="D12" t="n">
-        <v>4.0</v>
+        <v>2.0</v>
       </c>
       <c r="E12" t="n">
         <v>2.0</v>
       </c>
       <c r="F12" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G12" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H12" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="I12" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="J12" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="K12" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L12" t="n">
         <v>2.0</v>
       </c>
-      <c r="G12" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="H12" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="I12" t="n">
+      <c r="M12" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="N12" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="O12" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="P12" t="n">
         <v>3.0</v>
       </c>
-      <c r="J12" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="K12" t="n">
-        <v>5.0</v>
-      </c>
-      <c r="L12" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="M12" t="n">
+      <c r="Q12" t="n">
         <v>2.0</v>
-      </c>
-      <c r="N12" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="O12" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="P12" t="n">
-        <v>6.0</v>
-      </c>
-      <c r="Q12" t="n">
-        <v>3.0</v>
       </c>
       <c r="R12" t="n">
         <v>2.0</v>
       </c>
       <c r="S12" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="T12" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="U12" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="V12" t="n">
         <v>2.0</v>
       </c>
-      <c r="T12" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="U12" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="V12" t="n">
-        <v>1.0</v>
-      </c>
       <c r="W12" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X12" t="n">
         <v>2.0</v>
       </c>
-      <c r="X12" t="n">
-        <v>0.0</v>
-      </c>
       <c r="Y12" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="Z12" t="n">
         <v>2.0</v>
       </c>
     </row>
@@ -97255,76 +97390,73 @@
       <c r="B13" t="s">
         <v>30</v>
       </c>
-      <c r="C13" t="s">
-        <v>30</v>
+      <c r="C13" t="n">
+        <v>1.0</v>
       </c>
       <c r="D13" t="n">
-        <v>1.0</v>
+        <v>4.0</v>
       </c>
       <c r="E13" t="n">
         <v>4.0</v>
       </c>
       <c r="F13" t="n">
-        <v>4.0</v>
+        <v>3.0</v>
       </c>
       <c r="G13" t="n">
         <v>3.0</v>
       </c>
       <c r="H13" t="n">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
       <c r="I13" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="J13" t="n">
         <v>1.0</v>
       </c>
-      <c r="J13" t="n">
-        <v>4.0</v>
-      </c>
       <c r="K13" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="L13" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M13" t="n">
         <v>1.0</v>
-      </c>
-      <c r="L13" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="M13" t="n">
-        <v>0.0</v>
       </c>
       <c r="N13" t="n">
         <v>1.0</v>
       </c>
       <c r="O13" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="P13" t="n">
-        <v>3.0</v>
+        <v>7.0</v>
       </c>
       <c r="Q13" t="n">
-        <v>7.0</v>
+        <v>2.0</v>
       </c>
       <c r="R13" t="n">
         <v>2.0</v>
       </c>
       <c r="S13" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="T13" t="n">
         <v>2.0</v>
-      </c>
-      <c r="T13" t="n">
-        <v>1.0</v>
       </c>
       <c r="U13" t="n">
         <v>2.0</v>
       </c>
       <c r="V13" t="n">
-        <v>2.0</v>
+        <v>5.0</v>
       </c>
       <c r="W13" t="n">
         <v>5.0</v>
       </c>
       <c r="X13" t="n">
-        <v>5.0</v>
+        <v>4.0</v>
       </c>
       <c r="Y13" t="n">
-        <v>4.0</v>
-      </c>
-      <c r="Z13" t="n">
         <v>2.0</v>
       </c>
     </row>
@@ -97335,38 +97467,38 @@
       <c r="B14" t="s">
         <v>35</v>
       </c>
-      <c r="C14" t="s">
-        <v>35</v>
+      <c r="C14" t="n">
+        <v>1.0</v>
       </c>
       <c r="D14" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E14" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F14" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="G14" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H14" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I14" t="n">
         <v>1.0</v>
-      </c>
-      <c r="E14" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="F14" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="G14" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="H14" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="I14" t="n">
-        <v>0.0</v>
       </c>
       <c r="J14" t="n">
         <v>1.0</v>
       </c>
       <c r="K14" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="L14" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="M14" t="n">
         <v>1.0</v>
-      </c>
-      <c r="L14" t="n">
-        <v>4.0</v>
-      </c>
-      <c r="M14" t="n">
-        <v>2.0</v>
       </c>
       <c r="N14" t="n">
         <v>1.0</v>
@@ -97375,19 +97507,19 @@
         <v>1.0</v>
       </c>
       <c r="P14" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="Q14" t="n">
         <v>1.0</v>
       </c>
-      <c r="Q14" t="n">
-        <v>3.0</v>
-      </c>
       <c r="R14" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="S14" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="T14" t="n">
         <v>1.0</v>
-      </c>
-      <c r="S14" t="n">
-        <v>4.0</v>
-      </c>
-      <c r="T14" t="n">
-        <v>0.0</v>
       </c>
       <c r="U14" t="n">
         <v>1.0</v>
@@ -97396,15 +97528,12 @@
         <v>1.0</v>
       </c>
       <c r="W14" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="X14" t="n">
         <v>1.0</v>
       </c>
-      <c r="X14" t="n">
-        <v>2.0</v>
-      </c>
       <c r="Y14" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="Z14" t="n">
         <v>3.0</v>
       </c>
     </row>
@@ -97415,62 +97544,62 @@
       <c r="B15" t="s">
         <v>40</v>
       </c>
-      <c r="C15" t="s">
-        <v>40</v>
+      <c r="C15" t="n">
+        <v>1.0</v>
       </c>
       <c r="D15" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E15" t="n">
         <v>1.0</v>
       </c>
-      <c r="E15" t="n">
-        <v>0.0</v>
-      </c>
       <c r="F15" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="G15" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H15" t="n">
         <v>1.0</v>
       </c>
-      <c r="G15" t="n">
+      <c r="I15" t="n">
         <v>3.0</v>
       </c>
-      <c r="H15" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="I15" t="n">
+      <c r="J15" t="n">
         <v>1.0</v>
       </c>
-      <c r="J15" t="n">
-        <v>3.0</v>
-      </c>
       <c r="K15" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L15" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="M15" t="n">
         <v>1.0</v>
       </c>
-      <c r="L15" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="M15" t="n">
+      <c r="N15" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="O15" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="P15" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Q15" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="R15" t="n">
         <v>2.0</v>
       </c>
-      <c r="N15" t="n">
+      <c r="S15" t="n">
         <v>1.0</v>
       </c>
-      <c r="O15" t="n">
-        <v>4.0</v>
-      </c>
-      <c r="P15" t="n">
+      <c r="T15" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="U15" t="n">
         <v>1.0</v>
-      </c>
-      <c r="Q15" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="R15" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="S15" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="T15" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="U15" t="n">
-        <v>2.0</v>
       </c>
       <c r="V15" t="n">
         <v>1.0</v>
@@ -97479,12 +97608,9 @@
         <v>1.0</v>
       </c>
       <c r="X15" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="Y15" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="Z15" t="n">
         <v>0.0</v>
       </c>
     </row>
@@ -97495,62 +97621,62 @@
       <c r="B16" t="s">
         <v>33</v>
       </c>
-      <c r="C16" t="s">
-        <v>33</v>
+      <c r="C16" t="n">
+        <v>0.0</v>
       </c>
       <c r="D16" t="n">
-        <v>0.0</v>
+        <v>4.0</v>
       </c>
       <c r="E16" t="n">
-        <v>4.0</v>
+        <v>0.0</v>
       </c>
       <c r="F16" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="G16" t="n">
         <v>1.0</v>
       </c>
       <c r="H16" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="I16" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="J16" t="n">
         <v>1.0</v>
       </c>
-      <c r="I16" t="n">
-        <v>6.0</v>
-      </c>
-      <c r="J16" t="n">
-        <v>3.0</v>
-      </c>
       <c r="K16" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="L16" t="n">
         <v>1.0</v>
       </c>
-      <c r="L16" t="n">
-        <v>4.0</v>
-      </c>
       <c r="M16" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="N16" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="O16" t="n">
         <v>1.0</v>
-      </c>
-      <c r="N16" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="O16" t="n">
-        <v>0.0</v>
       </c>
       <c r="P16" t="n">
         <v>1.0</v>
       </c>
       <c r="Q16" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="R16" t="n">
         <v>1.0</v>
       </c>
-      <c r="R16" t="n">
+      <c r="S16" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="T16" t="n">
         <v>4.0</v>
       </c>
-      <c r="S16" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="T16" t="n">
-        <v>0.0</v>
-      </c>
       <c r="U16" t="n">
-        <v>4.0</v>
+        <v>2.0</v>
       </c>
       <c r="V16" t="n">
         <v>2.0</v>
@@ -97559,12 +97685,9 @@
         <v>2.0</v>
       </c>
       <c r="X16" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="Y16" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="Z16" t="n">
         <v>6.0</v>
       </c>
     </row>
@@ -97575,29 +97698,29 @@
       <c r="B17" t="s">
         <v>44</v>
       </c>
-      <c r="C17" t="s">
-        <v>44</v>
+      <c r="C17" t="n">
+        <v>5.0</v>
       </c>
       <c r="D17" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
       <c r="E17" t="n">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
       <c r="F17" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="G17" t="n">
         <v>1.0</v>
       </c>
       <c r="H17" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I17" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="J17" t="n">
         <v>1.0</v>
-      </c>
-      <c r="I17" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="J17" t="n">
-        <v>3.0</v>
       </c>
       <c r="K17" t="n">
         <v>1.0</v>
@@ -97606,13 +97729,13 @@
         <v>1.0</v>
       </c>
       <c r="M17" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="N17" t="n">
         <v>1.0</v>
       </c>
-      <c r="N17" t="n">
-        <v>0.0</v>
-      </c>
       <c r="O17" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="P17" t="n">
         <v>2.0</v>
@@ -97621,30 +97744,27 @@
         <v>2.0</v>
       </c>
       <c r="R17" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="S17" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="T17" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="U17" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="V17" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="W17" t="n">
         <v>2.0</v>
-      </c>
-      <c r="S17" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="T17" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="U17" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="V17" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="W17" t="n">
-        <v>0.0</v>
       </c>
       <c r="X17" t="n">
         <v>2.0</v>
       </c>
       <c r="Y17" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="Z17" t="n">
         <v>1.0</v>
       </c>
     </row>
@@ -97655,35 +97775,35 @@
       <c r="B18" t="s">
         <v>36</v>
       </c>
-      <c r="C18" t="s">
-        <v>36</v>
+      <c r="C18" t="n">
+        <v>1.0</v>
       </c>
       <c r="D18" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="E18" t="n">
         <v>2.0</v>
       </c>
       <c r="F18" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G18" t="n">
         <v>2.0</v>
       </c>
-      <c r="G18" t="n">
-        <v>0.0</v>
-      </c>
       <c r="H18" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="I18" t="n">
         <v>2.0</v>
-      </c>
-      <c r="I18" t="n">
-        <v>1.0</v>
       </c>
       <c r="J18" t="n">
         <v>2.0</v>
       </c>
       <c r="K18" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="L18" t="n">
         <v>2.0</v>
-      </c>
-      <c r="L18" t="n">
-        <v>1.0</v>
       </c>
       <c r="M18" t="n">
         <v>2.0</v>
@@ -97692,22 +97812,22 @@
         <v>2.0</v>
       </c>
       <c r="O18" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="P18" t="n">
         <v>2.0</v>
       </c>
-      <c r="P18" t="n">
+      <c r="Q18" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="R18" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="S18" t="n">
         <v>1.0</v>
       </c>
-      <c r="Q18" t="n">
+      <c r="T18" t="n">
         <v>2.0</v>
-      </c>
-      <c r="R18" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="S18" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="T18" t="n">
-        <v>1.0</v>
       </c>
       <c r="U18" t="n">
         <v>2.0</v>
@@ -97716,15 +97836,12 @@
         <v>2.0</v>
       </c>
       <c r="W18" t="n">
-        <v>2.0</v>
+        <v>0.0</v>
       </c>
       <c r="X18" t="n">
         <v>0.0</v>
       </c>
       <c r="Y18" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="Z18" t="n">
         <v>0.0</v>
       </c>
     </row>
@@ -97735,20 +97852,20 @@
       <c r="B19" t="s">
         <v>39</v>
       </c>
-      <c r="C19" t="s">
-        <v>39</v>
+      <c r="C19" t="n">
+        <v>1.0</v>
       </c>
       <c r="D19" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="E19" t="n">
         <v>1.0</v>
       </c>
-      <c r="E19" t="n">
+      <c r="F19" t="n">
         <v>2.0</v>
       </c>
-      <c r="F19" t="n">
+      <c r="G19" t="n">
         <v>1.0</v>
-      </c>
-      <c r="G19" t="n">
-        <v>2.0</v>
       </c>
       <c r="H19" t="n">
         <v>1.0</v>
@@ -97757,54 +97874,51 @@
         <v>1.0</v>
       </c>
       <c r="J19" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K19" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L19" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="M19" t="n">
         <v>1.0</v>
       </c>
-      <c r="K19" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="L19" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="M19" t="n">
+      <c r="N19" t="n">
         <v>2.0</v>
       </c>
-      <c r="N19" t="n">
+      <c r="O19" t="n">
         <v>1.0</v>
       </c>
-      <c r="O19" t="n">
+      <c r="P19" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Q19" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="R19" t="n">
         <v>2.0</v>
       </c>
-      <c r="P19" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="Q19" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="R19" t="n">
-        <v>0.0</v>
-      </c>
       <c r="S19" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="T19" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="U19" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="V19" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="W19" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="X19" t="n">
         <v>2.0</v>
       </c>
-      <c r="T19" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="U19" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="V19" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="W19" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="X19" t="n">
-        <v>4.0</v>
-      </c>
       <c r="Y19" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="Z19" t="n">
         <v>1.0</v>
       </c>
     </row>
@@ -97827,75 +97941,72 @@
         <v>85</v>
       </c>
       <c r="C1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="E1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="F1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="G1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="H1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="I1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="J1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="K1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="L1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="M1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="N1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="O1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="P1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="Q1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="R1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="S1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="T1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="U1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="V1" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="W1" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="X1" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="Y1" t="s">
-        <v>107</v>
-      </c>
-      <c r="Z1" t="s">
         <v>108</v>
       </c>
     </row>
@@ -97906,35 +98017,35 @@
       <c r="B2" t="s">
         <v>43</v>
       </c>
-      <c r="C2" t="s">
-        <v>43</v>
+      <c r="C2" t="n">
+        <v>4.0</v>
       </c>
       <c r="D2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E2" t="n">
         <v>4.0</v>
       </c>
-      <c r="E2" t="n">
-        <v>0.0</v>
-      </c>
       <c r="F2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H2" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="I2" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="J2" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="K2" t="n">
         <v>4.0</v>
       </c>
-      <c r="G2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="H2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="I2" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="J2" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="K2" t="n">
+      <c r="L2" t="n">
         <v>1.0</v>
-      </c>
-      <c r="L2" t="n">
-        <v>4.0</v>
       </c>
       <c r="M2" t="n">
         <v>1.0</v>
@@ -97946,36 +98057,33 @@
         <v>1.0</v>
       </c>
       <c r="P2" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="R2" t="n">
         <v>1.0</v>
       </c>
-      <c r="Q2" t="n">
+      <c r="S2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="T2" t="n">
         <v>3.0</v>
       </c>
-      <c r="R2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="S2" t="n">
+      <c r="U2" t="n">
         <v>1.0</v>
       </c>
-      <c r="T2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="U2" t="n">
+      <c r="V2" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="W2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X2" t="n">
         <v>3.0</v>
       </c>
-      <c r="V2" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="W2" t="n">
-        <v>5.0</v>
-      </c>
-      <c r="X2" t="n">
-        <v>0.0</v>
-      </c>
       <c r="Y2" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="Z2" t="n">
         <v>2.0</v>
       </c>
     </row>
@@ -97986,76 +98094,73 @@
       <c r="B3" t="s">
         <v>28</v>
       </c>
-      <c r="C3" t="s">
-        <v>28</v>
+      <c r="C3" t="n">
+        <v>1.0</v>
       </c>
       <c r="D3" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F3" t="n">
         <v>1.0</v>
       </c>
-      <c r="E3" t="n">
+      <c r="G3" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H3" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="I3" t="n">
         <v>2.0</v>
       </c>
-      <c r="F3" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="G3" t="n">
+      <c r="J3" t="n">
         <v>1.0</v>
       </c>
-      <c r="H3" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="I3" t="n">
+      <c r="K3" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L3" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="M3" t="n">
         <v>1.0</v>
       </c>
-      <c r="J3" t="n">
+      <c r="N3" t="n">
         <v>2.0</v>
       </c>
-      <c r="K3" t="n">
+      <c r="O3" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="P3" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="Q3" t="n">
         <v>1.0</v>
       </c>
-      <c r="L3" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="M3" t="n">
+      <c r="R3" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="S3" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="T3" t="n">
         <v>2.0</v>
       </c>
-      <c r="N3" t="n">
+      <c r="U3" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="V3" t="n">
         <v>1.0</v>
       </c>
-      <c r="O3" t="n">
+      <c r="W3" t="n">
         <v>2.0</v>
       </c>
-      <c r="P3" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="Q3" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="R3" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="S3" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="T3" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="U3" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="V3" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="W3" t="n">
-        <v>1.0</v>
-      </c>
       <c r="X3" t="n">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
       <c r="Y3" t="n">
-        <v>4.0</v>
-      </c>
-      <c r="Z3" t="n">
         <v>1.0</v>
       </c>
     </row>
@@ -98066,76 +98171,73 @@
       <c r="B4" t="s">
         <v>41</v>
       </c>
-      <c r="C4" t="s">
-        <v>41</v>
+      <c r="C4" t="n">
+        <v>0.0</v>
       </c>
       <c r="D4" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="E4" t="n">
         <v>1.0</v>
       </c>
       <c r="F4" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H4" t="n">
         <v>1.0</v>
       </c>
-      <c r="G4" t="n">
+      <c r="I4" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="J4" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="K4" t="n">
         <v>3.0</v>
       </c>
-      <c r="H4" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="I4" t="n">
+      <c r="L4" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="M4" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="N4" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="O4" t="n">
         <v>1.0</v>
-      </c>
-      <c r="J4" t="n">
-        <v>4.0</v>
-      </c>
-      <c r="K4" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="L4" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="M4" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="N4" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="O4" t="n">
-        <v>2.0</v>
       </c>
       <c r="P4" t="n">
         <v>1.0</v>
       </c>
       <c r="Q4" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="R4" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="S4" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="T4" t="n">
         <v>2.0</v>
-      </c>
-      <c r="S4" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="T4" t="n">
-        <v>0.0</v>
       </c>
       <c r="U4" t="n">
         <v>2.0</v>
       </c>
       <c r="V4" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="W4" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="X4" t="n">
         <v>2.0</v>
       </c>
-      <c r="W4" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="X4" t="n">
-        <v>1.0</v>
-      </c>
       <c r="Y4" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="Z4" t="n">
         <v>0.0</v>
       </c>
     </row>
@@ -98146,76 +98248,73 @@
       <c r="B5" t="s">
         <v>38</v>
       </c>
-      <c r="C5" t="s">
-        <v>38</v>
+      <c r="C5" t="n">
+        <v>1.0</v>
       </c>
       <c r="D5" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E5" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="F5" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="G5" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I5" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="J5" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K5" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L5" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="M5" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="N5" t="n">
         <v>1.0</v>
-      </c>
-      <c r="E5" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="F5" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="G5" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="H5" t="n">
-        <v>7.0</v>
-      </c>
-      <c r="I5" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="J5" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="K5" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="L5" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="M5" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="N5" t="n">
-        <v>0.0</v>
       </c>
       <c r="O5" t="n">
         <v>1.0</v>
       </c>
       <c r="P5" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="Q5" t="n">
         <v>1.0</v>
       </c>
-      <c r="Q5" t="n">
+      <c r="R5" t="n">
         <v>2.0</v>
       </c>
-      <c r="R5" t="n">
+      <c r="S5" t="n">
         <v>1.0</v>
       </c>
-      <c r="S5" t="n">
+      <c r="T5" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="U5" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="V5" t="n">
         <v>2.0</v>
       </c>
-      <c r="T5" t="n">
+      <c r="W5" t="n">
         <v>1.0</v>
       </c>
-      <c r="U5" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="V5" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="W5" t="n">
+      <c r="X5" t="n">
         <v>2.0</v>
       </c>
-      <c r="X5" t="n">
-        <v>1.0</v>
-      </c>
       <c r="Y5" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="Z5" t="n">
         <v>1.0</v>
       </c>
     </row>
@@ -98226,8 +98325,8 @@
       <c r="B6" t="s">
         <v>29</v>
       </c>
-      <c r="C6" t="s">
-        <v>29</v>
+      <c r="C6" t="n">
+        <v>2.0</v>
       </c>
       <c r="D6" t="n">
         <v>2.0</v>
@@ -98236,13 +98335,13 @@
         <v>2.0</v>
       </c>
       <c r="F6" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="G6" t="n">
         <v>2.0</v>
       </c>
-      <c r="G6" t="n">
-        <v>3.0</v>
-      </c>
       <c r="H6" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="I6" t="n">
         <v>1.0</v>
@@ -98254,48 +98353,45 @@
         <v>1.0</v>
       </c>
       <c r="L6" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M6" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="N6" t="n">
         <v>1.0</v>
-      </c>
-      <c r="M6" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="N6" t="n">
-        <v>2.0</v>
       </c>
       <c r="O6" t="n">
         <v>1.0</v>
       </c>
       <c r="P6" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="Q6" t="n">
         <v>1.0</v>
       </c>
-      <c r="Q6" t="n">
+      <c r="R6" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="S6" t="n">
         <v>3.0</v>
       </c>
-      <c r="R6" t="n">
+      <c r="T6" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="U6" t="n">
         <v>1.0</v>
       </c>
-      <c r="S6" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="T6" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="U6" t="n">
+      <c r="V6" t="n">
         <v>2.0</v>
       </c>
-      <c r="V6" t="n">
-        <v>1.0</v>
-      </c>
       <c r="W6" t="n">
-        <v>2.0</v>
+        <v>5.0</v>
       </c>
       <c r="X6" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
       <c r="Y6" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="Z6" t="n">
         <v>0.0</v>
       </c>
     </row>
@@ -98306,14 +98402,14 @@
       <c r="B7" t="s">
         <v>37</v>
       </c>
-      <c r="C7" t="s">
-        <v>37</v>
+      <c r="C7" t="n">
+        <v>5.0</v>
       </c>
       <c r="D7" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
       <c r="E7" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="F7" t="n">
         <v>1.0</v>
@@ -98328,43 +98424,43 @@
         <v>1.0</v>
       </c>
       <c r="J7" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="K7" t="n">
         <v>2.0</v>
       </c>
       <c r="L7" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="M7" t="n">
         <v>1.0</v>
       </c>
       <c r="N7" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="O7" t="n">
         <v>1.0</v>
       </c>
-      <c r="O7" t="n">
-        <v>0.0</v>
-      </c>
       <c r="P7" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="Q7" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="R7" t="n">
         <v>2.0</v>
       </c>
       <c r="S7" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="T7" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="U7" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="V7" t="n">
         <v>2.0</v>
-      </c>
-      <c r="T7" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="U7" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="V7" t="n">
-        <v>1.0</v>
       </c>
       <c r="W7" t="n">
         <v>2.0</v>
@@ -98373,9 +98469,6 @@
         <v>2.0</v>
       </c>
       <c r="Y7" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="Z7" t="n">
         <v>1.0</v>
       </c>
     </row>
@@ -98386,14 +98479,14 @@
       <c r="B8" t="s">
         <v>34</v>
       </c>
-      <c r="C8" t="s">
-        <v>34</v>
+      <c r="C8" t="n">
+        <v>1.0</v>
       </c>
       <c r="D8" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="E8" t="n">
         <v>1.0</v>
-      </c>
-      <c r="E8" t="n">
-        <v>3.0</v>
       </c>
       <c r="F8" t="n">
         <v>1.0</v>
@@ -98408,10 +98501,10 @@
         <v>1.0</v>
       </c>
       <c r="J8" t="n">
-        <v>1.0</v>
+        <v>5.0</v>
       </c>
       <c r="K8" t="n">
-        <v>5.0</v>
+        <v>2.0</v>
       </c>
       <c r="L8" t="n">
         <v>2.0</v>
@@ -98420,7 +98513,7 @@
         <v>2.0</v>
       </c>
       <c r="N8" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="O8" t="n">
         <v>1.0</v>
@@ -98429,33 +98522,30 @@
         <v>1.0</v>
       </c>
       <c r="Q8" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="R8" t="n">
         <v>2.0</v>
       </c>
       <c r="S8" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="T8" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="U8" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="V8" t="n">
         <v>2.0</v>
       </c>
-      <c r="T8" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="U8" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="V8" t="n">
-        <v>4.0</v>
-      </c>
       <c r="W8" t="n">
-        <v>2.0</v>
+        <v>0.0</v>
       </c>
       <c r="X8" t="n">
-        <v>0.0</v>
+        <v>3.0</v>
       </c>
       <c r="Y8" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="Z8" t="n">
         <v>0.0</v>
       </c>
     </row>
@@ -98466,38 +98556,38 @@
       <c r="B9" t="s">
         <v>31</v>
       </c>
-      <c r="C9" t="s">
-        <v>31</v>
+      <c r="C9" t="n">
+        <v>0.0</v>
       </c>
       <c r="D9" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="E9" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="F9" t="n">
         <v>1.0</v>
       </c>
-      <c r="F9" t="n">
-        <v>2.0</v>
-      </c>
       <c r="G9" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I9" t="n">
         <v>1.0</v>
-      </c>
-      <c r="H9" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="I9" t="n">
-        <v>0.0</v>
       </c>
       <c r="J9" t="n">
         <v>1.0</v>
       </c>
       <c r="K9" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L9" t="n">
         <v>1.0</v>
       </c>
-      <c r="L9" t="n">
-        <v>0.0</v>
-      </c>
       <c r="M9" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="N9" t="n">
         <v>2.0</v>
@@ -98506,36 +98596,33 @@
         <v>2.0</v>
       </c>
       <c r="P9" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Q9" t="n">
         <v>2.0</v>
       </c>
-      <c r="Q9" t="n">
-        <v>0.0</v>
-      </c>
       <c r="R9" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="S9" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="T9" t="n">
         <v>2.0</v>
       </c>
-      <c r="S9" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="T9" t="n">
+      <c r="U9" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="V9" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="W9" t="n">
         <v>1.0</v>
-      </c>
-      <c r="U9" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="V9" t="n">
-        <v>5.0</v>
-      </c>
-      <c r="W9" t="n">
-        <v>0.0</v>
       </c>
       <c r="X9" t="n">
         <v>1.0</v>
       </c>
       <c r="Y9" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="Z9" t="n">
         <v>1.0</v>
       </c>
     </row>
@@ -98546,76 +98633,73 @@
       <c r="B10" t="s">
         <v>45</v>
       </c>
-      <c r="C10" t="s">
-        <v>45</v>
+      <c r="C10" t="n">
+        <v>5.0</v>
       </c>
       <c r="D10" t="n">
-        <v>5.0</v>
+        <v>1.0</v>
       </c>
       <c r="E10" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="F10" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="G10" t="n">
         <v>2.0</v>
       </c>
       <c r="H10" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="I10" t="n">
         <v>3.0</v>
       </c>
       <c r="J10" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="K10" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="L10" t="n">
         <v>3.0</v>
       </c>
-      <c r="K10" t="n">
+      <c r="M10" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="N10" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="O10" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="P10" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="Q10" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="R10" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="S10" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="T10" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="U10" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="V10" t="n">
         <v>1.0</v>
       </c>
-      <c r="L10" t="n">
+      <c r="W10" t="n">
         <v>4.0</v>
       </c>
-      <c r="M10" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="N10" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="O10" t="n">
-        <v>4.0</v>
-      </c>
-      <c r="P10" t="n">
-        <v>6.0</v>
-      </c>
-      <c r="Q10" t="n">
-        <v>7.0</v>
-      </c>
-      <c r="R10" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="S10" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="T10" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="U10" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="V10" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="W10" t="n">
+      <c r="X10" t="n">
         <v>1.0</v>
       </c>
-      <c r="X10" t="n">
-        <v>4.0</v>
-      </c>
       <c r="Y10" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="Z10" t="n">
         <v>4.0</v>
       </c>
     </row>
@@ -98626,76 +98710,73 @@
       <c r="B11" t="s">
         <v>42</v>
       </c>
-      <c r="C11" t="s">
-        <v>42</v>
+      <c r="C11" t="n">
+        <v>3.0</v>
       </c>
       <c r="D11" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="E11" t="n">
-        <v>2.0</v>
+        <v>5.0</v>
       </c>
       <c r="F11" t="n">
-        <v>5.0</v>
+        <v>1.0</v>
       </c>
       <c r="G11" t="n">
         <v>1.0</v>
       </c>
       <c r="H11" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="I11" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="J11" t="n">
         <v>1.0</v>
       </c>
-      <c r="I11" t="n">
-        <v>6.0</v>
-      </c>
-      <c r="J11" t="n">
+      <c r="K11" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L11" t="n">
         <v>2.0</v>
       </c>
-      <c r="K11" t="n">
+      <c r="M11" t="n">
         <v>1.0</v>
       </c>
-      <c r="L11" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="M11" t="n">
+      <c r="N11" t="n">
         <v>2.0</v>
       </c>
-      <c r="N11" t="n">
+      <c r="O11" t="n">
         <v>1.0</v>
       </c>
-      <c r="O11" t="n">
+      <c r="P11" t="n">
         <v>2.0</v>
       </c>
-      <c r="P11" t="n">
+      <c r="Q11" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="R11" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="S11" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="T11" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="U11" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="V11" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="W11" t="n">
         <v>1.0</v>
       </c>
-      <c r="Q11" t="n">
+      <c r="X11" t="n">
         <v>2.0</v>
       </c>
-      <c r="R11" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="S11" t="n">
-        <v>4.0</v>
-      </c>
-      <c r="T11" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="U11" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="V11" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="W11" t="n">
-        <v>4.0</v>
-      </c>
-      <c r="X11" t="n">
-        <v>1.0</v>
-      </c>
       <c r="Y11" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="Z11" t="n">
         <v>6.0</v>
       </c>
     </row>
@@ -98706,76 +98787,73 @@
       <c r="B12" t="s">
         <v>32</v>
       </c>
-      <c r="C12" t="s">
-        <v>32</v>
+      <c r="C12" t="n">
+        <v>0.0</v>
       </c>
       <c r="D12" t="n">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
       <c r="E12" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F12" t="n">
         <v>2.0</v>
       </c>
-      <c r="F12" t="n">
+      <c r="G12" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H12" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="I12" t="n">
         <v>3.0</v>
       </c>
-      <c r="G12" t="n">
+      <c r="J12" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K12" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="L12" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M12" t="n">
         <v>2.0</v>
       </c>
-      <c r="H12" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="I12" t="n">
+      <c r="N12" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="O12" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="P12" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="Q12" t="n">
         <v>1.0</v>
       </c>
-      <c r="J12" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="K12" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="L12" t="n">
-        <v>4.0</v>
-      </c>
-      <c r="M12" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="N12" t="n">
+      <c r="R12" t="n">
         <v>2.0</v>
       </c>
-      <c r="O12" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="P12" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="Q12" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="R12" t="n">
+      <c r="S12" t="n">
         <v>1.0</v>
-      </c>
-      <c r="S12" t="n">
-        <v>2.0</v>
       </c>
       <c r="T12" t="n">
         <v>1.0</v>
       </c>
       <c r="U12" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="V12" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="W12" t="n">
         <v>2.0</v>
       </c>
-      <c r="W12" t="n">
-        <v>3.0</v>
-      </c>
       <c r="X12" t="n">
-        <v>2.0</v>
+        <v>0.0</v>
       </c>
       <c r="Y12" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="Z12" t="n">
         <v>1.0</v>
       </c>
     </row>
@@ -98786,53 +98864,53 @@
       <c r="B13" t="s">
         <v>30</v>
       </c>
-      <c r="C13" t="s">
-        <v>30</v>
+      <c r="C13" t="n">
+        <v>1.0</v>
       </c>
       <c r="D13" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E13" t="n">
         <v>1.0</v>
       </c>
-      <c r="E13" t="n">
-        <v>0.0</v>
-      </c>
       <c r="F13" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="G13" t="n">
         <v>1.0</v>
       </c>
-      <c r="G13" t="n">
-        <v>4.0</v>
-      </c>
       <c r="H13" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="I13" t="n">
         <v>0.0</v>
       </c>
       <c r="J13" t="n">
-        <v>0.0</v>
+        <v>5.0</v>
       </c>
       <c r="K13" t="n">
-        <v>5.0</v>
+        <v>2.0</v>
       </c>
       <c r="L13" t="n">
         <v>2.0</v>
       </c>
       <c r="M13" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="N13" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="O13" t="n">
         <v>1.0</v>
-      </c>
-      <c r="O13" t="n">
-        <v>0.0</v>
       </c>
       <c r="P13" t="n">
         <v>1.0</v>
       </c>
       <c r="Q13" t="n">
-        <v>1.0</v>
+        <v>5.0</v>
       </c>
       <c r="R13" t="n">
-        <v>5.0</v>
+        <v>2.0</v>
       </c>
       <c r="S13" t="n">
         <v>2.0</v>
@@ -98841,21 +98919,18 @@
         <v>2.0</v>
       </c>
       <c r="U13" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="V13" t="n">
         <v>1.0</v>
       </c>
       <c r="W13" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="X13" t="n">
         <v>2.0</v>
       </c>
       <c r="Y13" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="Z13" t="n">
         <v>3.0</v>
       </c>
     </row>
@@ -98866,32 +98941,32 @@
       <c r="B14" t="s">
         <v>35</v>
       </c>
-      <c r="C14" t="s">
-        <v>35</v>
+      <c r="C14" t="n">
+        <v>0.0</v>
       </c>
       <c r="D14" t="n">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
       <c r="E14" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F14" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G14" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H14" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="I14" t="n">
         <v>2.0</v>
       </c>
-      <c r="F14" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="G14" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="H14" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="I14" t="n">
+      <c r="J14" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="K14" t="n">
         <v>1.0</v>
-      </c>
-      <c r="J14" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="K14" t="n">
-        <v>3.0</v>
       </c>
       <c r="L14" t="n">
         <v>1.0</v>
@@ -98903,39 +98978,36 @@
         <v>1.0</v>
       </c>
       <c r="O14" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="P14" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Q14" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="R14" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="S14" t="n">
         <v>1.0</v>
       </c>
-      <c r="P14" t="n">
+      <c r="T14" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="U14" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="V14" t="n">
         <v>2.0</v>
       </c>
-      <c r="Q14" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="R14" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="S14" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="T14" t="n">
+      <c r="W14" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X14" t="n">
         <v>1.0</v>
       </c>
-      <c r="U14" t="n">
-        <v>4.0</v>
-      </c>
-      <c r="V14" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="W14" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="X14" t="n">
-        <v>0.0</v>
-      </c>
       <c r="Y14" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="Z14" t="n">
         <v>2.0</v>
       </c>
     </row>
@@ -98946,26 +99018,26 @@
       <c r="B15" t="s">
         <v>40</v>
       </c>
-      <c r="C15" t="s">
-        <v>40</v>
+      <c r="C15" t="n">
+        <v>1.0</v>
       </c>
       <c r="D15" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="E15" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="F15" t="n">
         <v>1.0</v>
-      </c>
-      <c r="E15" t="n">
-        <v>4.0</v>
-      </c>
-      <c r="F15" t="n">
-        <v>2.0</v>
       </c>
       <c r="G15" t="n">
         <v>1.0</v>
       </c>
       <c r="H15" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I15" t="n">
         <v>1.0</v>
-      </c>
-      <c r="I15" t="n">
-        <v>0.0</v>
       </c>
       <c r="J15" t="n">
         <v>1.0</v>
@@ -98980,42 +99052,39 @@
         <v>1.0</v>
       </c>
       <c r="N15" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="O15" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="P15" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="Q15" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="R15" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="S15" t="n">
         <v>1.0</v>
-      </c>
-      <c r="O15" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="P15" t="n">
-        <v>4.0</v>
-      </c>
-      <c r="Q15" t="n">
-        <v>6.0</v>
-      </c>
-      <c r="R15" t="n">
-        <v>4.0</v>
-      </c>
-      <c r="S15" t="n">
-        <v>3.0</v>
       </c>
       <c r="T15" t="n">
         <v>1.0</v>
       </c>
       <c r="U15" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="V15" t="n">
         <v>2.0</v>
       </c>
       <c r="W15" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="X15" t="n">
         <v>2.0</v>
       </c>
-      <c r="X15" t="n">
-        <v>1.0</v>
-      </c>
       <c r="Y15" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="Z15" t="n">
         <v>6.0</v>
       </c>
     </row>
@@ -99026,29 +99095,29 @@
       <c r="B16" t="s">
         <v>33</v>
       </c>
-      <c r="C16" t="s">
-        <v>33</v>
+      <c r="C16" t="n">
+        <v>1.0</v>
       </c>
       <c r="D16" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E16" t="n">
         <v>1.0</v>
       </c>
-      <c r="E16" t="n">
-        <v>0.0</v>
-      </c>
       <c r="F16" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="G16" t="n">
         <v>1.0</v>
       </c>
-      <c r="G16" t="n">
-        <v>4.0</v>
-      </c>
       <c r="H16" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I16" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="J16" t="n">
         <v>1.0</v>
-      </c>
-      <c r="I16" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="J16" t="n">
-        <v>0.0</v>
       </c>
       <c r="K16" t="n">
         <v>1.0</v>
@@ -99060,42 +99129,39 @@
         <v>1.0</v>
       </c>
       <c r="N16" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="O16" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="P16" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="Q16" t="n">
         <v>1.0</v>
-      </c>
-      <c r="O16" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="P16" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="Q16" t="n">
-        <v>2.0</v>
       </c>
       <c r="R16" t="n">
         <v>1.0</v>
       </c>
       <c r="S16" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="T16" t="n">
         <v>1.0</v>
       </c>
-      <c r="T16" t="n">
-        <v>2.0</v>
-      </c>
       <c r="U16" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="V16" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="W16" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="X16" t="n">
         <v>1.0</v>
       </c>
-      <c r="V16" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="W16" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="X16" t="n">
-        <v>3.0</v>
-      </c>
       <c r="Y16" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="Z16" t="n">
         <v>1.0</v>
       </c>
     </row>
@@ -99106,26 +99172,26 @@
       <c r="B17" t="s">
         <v>44</v>
       </c>
-      <c r="C17" t="s">
-        <v>44</v>
+      <c r="C17" t="n">
+        <v>1.0</v>
       </c>
       <c r="D17" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="E17" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F17" t="n">
         <v>1.0</v>
       </c>
-      <c r="E17" t="n">
-        <v>4.0</v>
-      </c>
-      <c r="F17" t="n">
+      <c r="G17" t="n">
         <v>3.0</v>
       </c>
-      <c r="G17" t="n">
+      <c r="H17" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I17" t="n">
         <v>1.0</v>
-      </c>
-      <c r="H17" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="I17" t="n">
-        <v>0.0</v>
       </c>
       <c r="J17" t="n">
         <v>1.0</v>
@@ -99134,48 +99200,45 @@
         <v>1.0</v>
       </c>
       <c r="L17" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="M17" t="n">
         <v>1.0</v>
       </c>
-      <c r="M17" t="n">
-        <v>4.0</v>
-      </c>
       <c r="N17" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="O17" t="n">
         <v>1.0</v>
       </c>
-      <c r="O17" t="n">
+      <c r="P17" t="n">
         <v>2.0</v>
       </c>
-      <c r="P17" t="n">
+      <c r="Q17" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="R17" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="S17" t="n">
         <v>1.0</v>
       </c>
-      <c r="Q17" t="n">
+      <c r="T17" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="U17" t="n">
         <v>2.0</v>
-      </c>
-      <c r="R17" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="S17" t="n">
-        <v>5.0</v>
-      </c>
-      <c r="T17" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="U17" t="n">
-        <v>0.0</v>
       </c>
       <c r="V17" t="n">
         <v>2.0</v>
       </c>
       <c r="W17" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="X17" t="n">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
       <c r="Y17" t="n">
-        <v>4.0</v>
-      </c>
-      <c r="Z17" t="n">
         <v>1.0</v>
       </c>
     </row>
@@ -99186,76 +99249,73 @@
       <c r="B18" t="s">
         <v>36</v>
       </c>
-      <c r="C18" t="s">
-        <v>36</v>
+      <c r="C18" t="n">
+        <v>1.0</v>
       </c>
       <c r="D18" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="E18" t="n">
         <v>1.0</v>
       </c>
-      <c r="E18" t="n">
+      <c r="F18" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G18" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="H18" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I18" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="J18" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K18" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="L18" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="M18" t="n">
         <v>2.0</v>
       </c>
-      <c r="F18" t="n">
+      <c r="N18" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="O18" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="P18" t="n">
         <v>1.0</v>
-      </c>
-      <c r="G18" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="H18" t="n">
-        <v>4.0</v>
-      </c>
-      <c r="I18" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="J18" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="K18" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="L18" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="M18" t="n">
-        <v>5.0</v>
-      </c>
-      <c r="N18" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="O18" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="P18" t="n">
-        <v>2.0</v>
       </c>
       <c r="Q18" t="n">
         <v>1.0</v>
       </c>
       <c r="R18" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="S18" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="T18" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="U18" t="n">
         <v>1.0</v>
-      </c>
-      <c r="S18" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="T18" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="U18" t="n">
-        <v>2.0</v>
       </c>
       <c r="V18" t="n">
         <v>1.0</v>
       </c>
       <c r="W18" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="X18" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="Y18" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="Z18" t="n">
         <v>1.0</v>
       </c>
     </row>
@@ -99266,76 +99326,73 @@
       <c r="B19" t="s">
         <v>39</v>
       </c>
-      <c r="C19" t="s">
-        <v>39</v>
+      <c r="C19" t="n">
+        <v>0.0</v>
       </c>
       <c r="D19" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="E19" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F19" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G19" t="n">
         <v>1.0</v>
       </c>
-      <c r="F19" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="G19" t="n">
-        <v>0.0</v>
-      </c>
       <c r="H19" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="I19" t="n">
         <v>3.0</v>
       </c>
       <c r="J19" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="K19" t="n">
         <v>2.0</v>
       </c>
       <c r="L19" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M19" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="N19" t="n">
         <v>2.0</v>
       </c>
-      <c r="M19" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="N19" t="n">
-        <v>0.0</v>
-      </c>
       <c r="O19" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="P19" t="n">
         <v>3.0</v>
       </c>
       <c r="Q19" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="R19" t="n">
         <v>3.0</v>
       </c>
-      <c r="R19" t="n">
+      <c r="S19" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="T19" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="U19" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="V19" t="n">
         <v>2.0</v>
       </c>
-      <c r="S19" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="T19" t="n">
-        <v>4.0</v>
-      </c>
-      <c r="U19" t="n">
+      <c r="W19" t="n">
         <v>1.0</v>
       </c>
-      <c r="V19" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="W19" t="n">
-        <v>2.0</v>
-      </c>
       <c r="X19" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="Y19" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="Z19" t="n">
         <v>2.0</v>
       </c>
     </row>
@@ -99417,6 +99474,15 @@
       <c r="V1" t="s">
         <v>105</v>
       </c>
+      <c r="W1" t="s">
+        <v>106</v>
+      </c>
+      <c r="X1" t="s">
+        <v>107</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
@@ -99485,6 +99551,15 @@
       <c r="V2" t="n">
         <v>6.0</v>
       </c>
+      <c r="W2" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="X2" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="Y2" t="n">
+        <v>3.0</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
@@ -99553,6 +99628,15 @@
       <c r="V3" t="n">
         <v>5.0</v>
       </c>
+      <c r="W3" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="X3" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="Y3" t="n">
+        <v>5.0</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
@@ -99621,6 +99705,15 @@
       <c r="V4" t="n">
         <v>2.0</v>
       </c>
+      <c r="W4" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="X4" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="Y4" t="n">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
@@ -99689,6 +99782,15 @@
       <c r="V5" t="n">
         <v>4.0</v>
       </c>
+      <c r="W5" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="X5" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="Y5" t="n">
+        <v>2.0</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
@@ -99757,6 +99859,15 @@
       <c r="V6" t="n">
         <v>5.0</v>
       </c>
+      <c r="W6" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="X6" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="Y6" t="n">
+        <v>6.0</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
@@ -99825,6 +99936,15 @@
       <c r="V7" t="n">
         <v>2.0</v>
       </c>
+      <c r="W7" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="X7" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="Y7" t="n">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
@@ -99893,6 +100013,15 @@
       <c r="V8" t="n">
         <v>4.0</v>
       </c>
+      <c r="W8" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="X8" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="Y8" t="n">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
@@ -99961,6 +100090,15 @@
       <c r="V9" t="n">
         <v>2.0</v>
       </c>
+      <c r="W9" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="X9" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="Y9" t="n">
+        <v>3.0</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
@@ -100029,6 +100167,15 @@
       <c r="V10" t="n">
         <v>3.0</v>
       </c>
+      <c r="W10" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="X10" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="Y10" t="n">
+        <v>5.0</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
@@ -100097,6 +100244,15 @@
       <c r="V11" t="n">
         <v>5.0</v>
       </c>
+      <c r="W11" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="X11" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="Y11" t="n">
+        <v>7.0</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
@@ -100165,6 +100321,15 @@
       <c r="V12" t="n">
         <v>5.0</v>
       </c>
+      <c r="W12" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="X12" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="Y12" t="n">
+        <v>3.0</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
@@ -100233,6 +100398,15 @@
       <c r="V13" t="n">
         <v>6.0</v>
       </c>
+      <c r="W13" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="X13" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="Y13" t="n">
+        <v>5.0</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
@@ -100301,6 +100475,15 @@
       <c r="V14" t="n">
         <v>3.0</v>
       </c>
+      <c r="W14" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="X14" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="Y14" t="n">
+        <v>5.0</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
@@ -100369,6 +100552,15 @@
       <c r="V15" t="n">
         <v>3.0</v>
       </c>
+      <c r="W15" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="X15" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="Y15" t="n">
+        <v>6.0</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
@@ -100437,6 +100629,15 @@
       <c r="V16" t="n">
         <v>2.0</v>
       </c>
+      <c r="W16" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="X16" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="Y16" t="n">
+        <v>7.0</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
@@ -100505,6 +100706,15 @@
       <c r="V17" t="n">
         <v>2.0</v>
       </c>
+      <c r="W17" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="X17" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="Y17" t="n">
+        <v>2.0</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
@@ -100573,6 +100783,15 @@
       <c r="V18" t="n">
         <v>3.0</v>
       </c>
+      <c r="W18" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="X18" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="Y18" t="n">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
@@ -100640,6 +100859,15 @@
       </c>
       <c r="V19" t="n">
         <v>2.0</v>
+      </c>
+      <c r="W19" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="X19" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="Y19" t="n">
+        <v>3.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>